<commit_message>
Aula 10 - Importando arquivos Html - primeiro controller criado e endpoint testado
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>aula</t>
   </si>
@@ -38,13 +38,28 @@
     <t>observação</t>
   </si>
   <si>
-    <t>2-Iniciando o desenvolvimento do projeto</t>
-  </si>
-  <si>
     <t>Criando o projeto via wizard do STS</t>
   </si>
   <si>
     <t>4:50 - adicionar os pacotes iniciais de projeto: DevTools, Thymeleaf e Spring Web</t>
+  </si>
+  <si>
+    <t>2. Inciando o Desenvolvimento do Projeto</t>
+  </si>
+  <si>
+    <t>10. Importanto os arquivos HTML</t>
+  </si>
+  <si>
+    <t>2. Iniciando o desenvolvimento do projeto</t>
+  </si>
+  <si>
+    <t>2:53
+por padrão, as paginas HTML devem ficar no diretório TEMPLATES pois é lá que o spring MVC procura as páginas. Caso deseja alterar esse diretório padrão, é necessário sobrescrever o arquivo de propriedades do thymeleaf (professor citou que isso será visto em aulas posteriores)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4:35
+O spring MVC só encontra as páginas HTML através de um CONTROLLER
+</t>
   </si>
 </sst>
 </file>
@@ -80,8 +95,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E3"/>
+  <dimension ref="B2:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,13 +412,41 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="4" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aula 11 - Incluindo Recursos WebJars - estilizando paginas com dependencias jquery e bootstrap
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>aula</t>
   </si>
@@ -60,14 +60,28 @@
     <t xml:space="preserve">4:35
 O spring MVC só encontra as páginas HTML através de um CONTROLLER
 </t>
+  </si>
+  <si>
+    <t>11. Incluíndo o recurso de WebJars</t>
+  </si>
+  <si>
+    <t>6:08 - foi ensinado uma forma de adicionar bibliotecas para pagina HTML (Jquery, bootstrap, icones) através de dependências no pom.xml. Usando esta forma, o "src" do documento html deve direcionar para o diretorio raiz onde encontra-se os webjars baixados pelo pom. É possivel ver o local destes diretórios direto na documentação das bibliotecas. Os webjars podem ser baixados atraves do site https://www.webjars.org/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -95,11 +109,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E5"/>
+  <dimension ref="B2:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +464,25 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Aula 12 - Testando os links do menu - primeiros endpoints para acesso ao cadastro e lista de funcionario, cargo e departamento
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>aula</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>4:50 - adicionar os pacotes iniciais de projeto: DevTools, Thymeleaf e Spring Web</t>
-  </si>
-  <si>
-    <t>2. Inciando o Desenvolvimento do Projeto</t>
   </si>
   <si>
     <t>10. Importanto os arquivos HTML</t>
@@ -66,22 +63,20 @@
   </si>
   <si>
     <t>6:08 - foi ensinado uma forma de adicionar bibliotecas para pagina HTML (Jquery, bootstrap, icones) através de dependências no pom.xml. Usando esta forma, o "src" do documento html deve direcionar para o diretorio raiz onde encontra-se os webjars baixados pelo pom. É possivel ver o local destes diretórios direto na documentação das bibliotecas. Os webjars podem ser baixados atraves do site https://www.webjars.org/</t>
+  </si>
+  <si>
+    <t>Testando os links do menu</t>
+  </si>
+  <si>
+    <t>Nesta aula foi criado os primeiros endpoints para acesso dos menus de cadastro e lista de funcionario, cargos e departamentos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -114,7 +109,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,7 +395,7 @@
   <dimension ref="B2:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,7 +424,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -441,13 +438,13 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="75" x14ac:dyDescent="0.25">
@@ -455,13 +452,13 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="90" x14ac:dyDescent="0.25">
@@ -469,17 +466,28 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="1" t="s">
+    </row>
+    <row r="7" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E7" s="2"/>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Aula 14 - Adicionando o Starter para JPA - uma unica dependencia do spring capaz de baixar todo pacote JPA
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>aula</t>
   </si>
@@ -69,6 +69,22 @@
   </si>
   <si>
     <t>Nesta aula foi criado os primeiros endpoints para acesso dos menus de cadastro e lista de funcionario, cargos e departamentos</t>
+  </si>
+  <si>
+    <t>3. Classes de Domínio</t>
+  </si>
+  <si>
+    <t>14. Adicionando o Starter para JPA</t>
+  </si>
+  <si>
+    <t>SOMENTE RESUMO</t>
+  </si>
+  <si>
+    <t>4:52 - adicao de dependencia referente ao STARTER JPA/HIBERNATE... ao adicionar a dependencia abaixo, o maven baixa um pacotao de dependencias basicas e necessários para acesso ao banco de dados por JPA/HIBERNATE
+&lt;dependency&gt;
+&lt;groupId&gt;org.springframework.boot&lt;/groupId&gt;
+&lt;artifactId&gt;spring-boot-starter-data-jpa&lt;/artifactId&gt;
+&lt;/dependency&gt;</t>
   </si>
 </sst>
 </file>
@@ -392,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E7"/>
+  <dimension ref="B2:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,6 +505,34 @@
         <v>13</v>
       </c>
     </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aula 15 - Super Classe para Entidades - uma classe abstrata que tem a funcao de eliminar a necessidade de declarar ids nas entidades
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>aula</t>
   </si>
@@ -85,6 +85,12 @@
 &lt;groupId&gt;org.springframework.boot&lt;/groupId&gt;
 &lt;artifactId&gt;spring-boot-starter-data-jpa&lt;/artifactId&gt;
 &lt;/dependency&gt;</t>
+  </si>
+  <si>
+    <t>15. Super Classe para Entidades</t>
+  </si>
+  <si>
+    <t>4:43 - criação de uma classe abstrata para ser usada como herança, tem a função de eliminar a necessidade de declarar/setar ids nas entidades. Para seu uso, ao implementar a entidade é necessário colocar a instrução "extends" herdando assim a classe abstrata passando como parametro um tipo LONG</t>
   </si>
 </sst>
 </file>
@@ -408,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E9"/>
+  <dimension ref="B2:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,6 +539,20 @@
         <v>17</v>
       </c>
     </row>
+    <row r="10" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aula 16 - As entidades Departamento e Cargo (somente criacao, sem testes)
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>aula</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>4:43 - criação de uma classe abstrata para ser usada como herança, tem a função de eliminar a necessidade de declarar/setar ids nas entidades. Para seu uso, ao implementar a entidade é necessário colocar a instrução "extends" herdando assim a classe abstrata passando como parametro um tipo LONG</t>
+  </si>
+  <si>
+    <t>16. As entidades Departamento e Cargo</t>
+  </si>
+  <si>
+    <t>6:04 - relacionamento bidirecional, neste caso usa-se a anotação @OneToMany com o atributo mappedBy apontando para a tabela mais forte. É obrigatório definir quem é lado fraco e o lado forte da relação. A tabela mais forte é o lado que tem/gera a chave estrangeira, neste caso CARGO.</t>
   </si>
 </sst>
 </file>
@@ -414,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E10"/>
+  <dimension ref="B2:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,6 +559,20 @@
         <v>19</v>
       </c>
     </row>
+    <row r="11" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aula 17 - A entidade Endereco (somente criacao, sem testes)
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>aula</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>6:04 - relacionamento bidirecional, neste caso usa-se a anotação @OneToMany com o atributo mappedBy apontando para a tabela mais forte. É obrigatório definir quem é lado fraco e o lado forte da relação. A tabela mais forte é o lado que tem/gera a chave estrangeira, neste caso CARGO.</t>
+  </si>
+  <si>
+    <t>17. A entidade Endereco</t>
+  </si>
+  <si>
+    <t>3:48 - anotação @Enumerated, que define na entidade, informando para o JPA qual o tipo de dado deve ser armazenado no banco de dados com o atributo EnumType.String, salvando um enum com o tipo string</t>
   </si>
 </sst>
 </file>
@@ -420,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E11"/>
+  <dimension ref="B2:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14:E17"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,6 +579,20 @@
         <v>21</v>
       </c>
     </row>
+    <row r="12" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aula 22 - Incluindo os DAOs especificos
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>aula</t>
   </si>
@@ -103,6 +103,15 @@
   </si>
   <si>
     <t>3:48 - anotação @Enumerated, que define na entidade, informando para o JPA qual o tipo de dado deve ser armazenado no banco de dados com o atributo EnumType.String, salvando um enum com o tipo string</t>
+  </si>
+  <si>
+    <t>criado repositorys e daos de forma diferente ao que foi abordado em outro curso</t>
+  </si>
+  <si>
+    <t>22. Incluindo DAO'S especificos</t>
+  </si>
+  <si>
+    <t>4. Camada de Persistência</t>
   </si>
 </sst>
 </file>
@@ -426,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E12"/>
+  <dimension ref="B2:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,6 +602,20 @@
         <v>23</v>
       </c>
     </row>
+    <row r="13" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aula 25 - Incluindo Services - inicio da implementacao do pacote e classes services
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>aula</t>
   </si>
@@ -113,15 +113,38 @@
   <si>
     <t>4. Camada de Persistência</t>
   </si>
+  <si>
+    <t>5. Camada de Serviço</t>
+  </si>
+  <si>
+    <t>24. Gerenciamento de Transações</t>
+  </si>
+  <si>
+    <t>0:36 - IMPORTANTE: anotação @Transactional; é utilizada tanto sobre a assinatura de uma classe como a assinatura de um método. Para gerenciar transaçoes pelo spring é utilizada esta anotação. A anotação possui um atributo chamada "readonly"... um booleano que define se vai precisar que uma transação seja aberta ou não. Quando uma transação é aberta, isso bloqueia o a tabela para outros usuários para operações como metodos de insert, update, delete. Portanto isso pode ser interessante para definir em metodos somente de leitura de dados.</t>
+  </si>
+  <si>
+    <t>25. Incluindo Services</t>
+  </si>
+  <si>
+    <t>nenhuma anotação na aula porém foi o inicio da implementação dos serviçes, das interfaces e como elas agem. Interessante revisar caso sugir duvidas</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -147,12 +170,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -435,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E13"/>
+  <dimension ref="B2:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,6 +643,34 @@
         <v>24</v>
       </c>
     </row>
+    <row r="14" spans="2:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="B14" s="3">
+        <v>24</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aula 26 - Finalizando services - para departamento e funcionario
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t>aula</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>nenhuma anotação na aula porém foi o inicio da implementação dos serviçes, das interfaces e como elas agem. Interessante revisar caso sugir duvidas</t>
+  </si>
+  <si>
+    <t>27. RESUMO</t>
+  </si>
+  <si>
+    <t>Não tem video porém tem um resumo interessante com mais detalhes sobre a anotação @Transactional e exemplos de uso, vale a pena a leitura</t>
   </si>
 </sst>
 </file>
@@ -462,17 +468,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E15"/>
+  <dimension ref="B2:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="39.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="74.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="74.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
@@ -671,6 +677,20 @@
         <v>31</v>
       </c>
     </row>
+    <row r="16" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aula 29 - Incluindo o Thymeleaf-layout - dependencia e alteracao do application.properties
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
   <si>
     <t>aula</t>
   </si>
@@ -133,6 +133,23 @@
   </si>
   <si>
     <t>Não tem video porém tem um resumo interessante com mais detalhes sobre a anotação @Transactional e exemplos de uso, vale a pena a leitura</t>
+  </si>
+  <si>
+    <t>5:56 - abordado chaves e configurações que podem ser inseridas no application.properties para mais configurações do thymeleaf. O próprio spring boot ja pré-configura algumas coisas do thymeleaf, mas caso não seja usado o spring boot, podem ser feitas estas alterações direto no projeto, como por exemplo o prefixo de paginas citado em aulas anteriores, que é o diretorio onde fica localizado os arquivos .html do front-end. Mais detalhes na documentação descrita no link: https://docs.spring.io/spring-boot/docs/current/reference/htmlsingle/</t>
+  </si>
+  <si>
+    <t>7. Thymeleaf para as Views</t>
+  </si>
+  <si>
+    <t>29. Incluindo o Thymeleaf-Layout</t>
+  </si>
+  <si>
+    <t>5:03
+inclusão de dependencia para uso de templates no thymeleaf
+&lt;dependency&gt;
+&lt;groupId&gt;nz.net.ultraq.thymeleaf&lt;/groupId&gt;
+&lt;artifactId&gt;thymeleaf-layout-dialect&lt;/artifactId&gt;
+&lt;/dependency&gt;</t>
   </si>
 </sst>
 </file>
@@ -468,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E16"/>
+  <dimension ref="B2:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,6 +708,34 @@
         <v>33</v>
       </c>
     </row>
+    <row r="17" spans="2:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aula 30 - Template baseado em layout - Criacao do layout.html, modelo basico para compor todas paginas
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
   <si>
     <t>aula</t>
   </si>
@@ -150,6 +150,28 @@
 &lt;groupId&gt;nz.net.ultraq.thymeleaf&lt;/groupId&gt;
 &lt;artifactId&gt;thymeleaf-layout-dialect&lt;/artifactId&gt;
 &lt;/dependency&gt;</t>
+  </si>
+  <si>
+    <t>30. Template baseado em layout</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2:50 - para criar templeate baseado em layout, o template modelo HTML do thymeleaf deve conter os namespaces necessários a seguir;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+xmlns:th="http://www.thymeleaf.org"
+xmlns:layout="http://www.ultraq.net.nz/thymeleaf/layout"</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -485,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E18"/>
+  <dimension ref="B2:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E23" sqref="E23:E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,6 +758,20 @@
         <v>37</v>
       </c>
     </row>
+    <row r="19" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aula 32 - Fragmentando o cabeçalho e rodape
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
   <si>
     <t>aula</t>
   </si>
@@ -172,6 +172,41 @@
 xmlns:th="http://www.thymeleaf.org"
 xmlns:layout="http://www.ultraq.net.nz/thymeleaf/layout"</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">nenhum código foi criado, porém explica de forma bem didática e detalhada o funcionamento e a aplicação de fragmentos em paginas HTML. No meu entendimento, fragments são pedaços ou componentes de codigos em documentos HTML que usando as tags de acordo, podem ser reaproveitadas em outras páginas. Existêm 3 formas de reaproveitamento que são: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT, INCLUDE e REPLACE.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Cada um terá um comportamento diferente na página de destino. INSERT inclui a tag inteira e seu conteudo. REPLACE substitui o componente pai e insere somente o componente do fragmento. REPLACE ignora a tag pai e a tag do fragmento e insere somente o seu VALOR/CONTEUDO.</t>
+    </r>
+  </si>
+  <si>
+    <t>31. O Processo de fragmentação</t>
+  </si>
+  <si>
+    <t>32 . Fragmentando o cabeçalho e rodapé</t>
+  </si>
+  <si>
+    <t>mostra na prática como é feito o processo de fragmentação, como é feito a chamada entre documentos HTML usando tag do thymeleaf</t>
   </si>
 </sst>
 </file>
@@ -507,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E19"/>
+  <dimension ref="B2:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23:E26"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,6 +807,34 @@
         <v>39</v>
       </c>
     </row>
+    <row r="20" spans="2:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>32</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aula 33 - Fragmentando o sidebar e a pagina home - utilizacao de novo recurso para fragmento
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
   <si>
     <t>aula</t>
   </si>
@@ -207,6 +207,18 @@
   </si>
   <si>
     <t>mostra na prática como é feito o processo de fragmentação, como é feito a chamada entre documentos HTML usando tag do thymeleaf</t>
+  </si>
+  <si>
+    <t>1:28
+7. Thymeleaf para as Views
+32. Fragmentando o cabeçalho e rodapé
+para usar os componentes do thymeleaf na IDE, é interessante habilitar o plugin para que a IDE reconheça e faça o auto preenchimento. Para habilitar utilizando o a ide STS basta clicar direito com direito em cima do projeto, ir em Thymeleaf e clicar em Add Thymeleaf Nature</t>
+  </si>
+  <si>
+    <t>33. Fragmentando o sidebar e a página home</t>
+  </si>
+  <si>
+    <t>2:36 - aplicando fragmento através da biblioteca de layout o "layout:fragment" invés do th:fragment do thymeleaf. a biblioteca layout:fragment fornece recursos mais avançados.</t>
   </si>
 </sst>
 </file>
@@ -542,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E21"/>
+  <dimension ref="B2:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,6 +847,34 @@
         <v>43</v>
       </c>
     </row>
+    <row r="22" spans="2:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>32</v>
+      </c>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>33</v>
+      </c>
+      <c r="C23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aula 34 - Fragmentando paginas de cadastros e listagens
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
   <si>
     <t>aula</t>
   </si>
@@ -219,6 +219,19 @@
   </si>
   <si>
     <t>2:36 - aplicando fragmento através da biblioteca de layout o "layout:fragment" invés do th:fragment do thymeleaf. a biblioteca layout:fragment fornece recursos mais avançados.</t>
+  </si>
+  <si>
+    <t>34. Fragmentando páginas de cadastros e listagens</t>
+  </si>
+  <si>
+    <t>demonstra na pratica como fragmentar as demais páginas usando o layout:fragment e layout:decorate</t>
+  </si>
+  <si>
+    <t>RESUMO</t>
+  </si>
+  <si>
+    <t>Um resumão sobre tudo que foi aprendido na sessão/módulo/capitulo
+a leitura é valida caso surja dúvidas</t>
   </si>
 </sst>
 </file>
@@ -554,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E23"/>
+  <dimension ref="B2:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,11 +881,39 @@
       <c r="C23" t="s">
         <v>35</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>34</v>
+      </c>
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>35</v>
+      </c>
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aula 36 - Inserindo departamentos
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="58">
   <si>
     <t>aula</t>
   </si>
@@ -232,6 +232,32 @@
   <si>
     <t>Um resumão sobre tudo que foi aprendido na sessão/módulo/capitulo
 a leitura é valida caso surja dúvidas</t>
+  </si>
+  <si>
+    <t>8. Departamento: Controller &amp; View</t>
+  </si>
+  <si>
+    <t>36. Inserindo departamentos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+2:12 - aplicação de chamada de endpoint atraves de tags e expressões do Thymeleaf. a expressão utilizada para o thymeleaf é "@{/seu/endpoit/aqui}" ... o parêntese permanece no código.</t>
+  </si>
+  <si>
+    <t>3:32
+declaração de váriavel do thymeleaf no documento HTML com a expressão: th:object="${departamento}". Essa variável podera ser acessada pelo backend, como por exemplo acessar objetos da entidade. ela tem ligação direta com outra expressão do thymeleaf chamada th:field="*{nomeDoAtributoDoObjetoAqui}"</t>
+  </si>
+  <si>
+    <t>4:30
+declaração de atributo do thymeleaf no documento HTML, diferente de variavel, o th:field="*{nomeDoAtributoDoObjetoAqui}"tem ligação direta com o th:object. Com o th:field é possível acessar os atributos de uma classe.</t>
+  </si>
+  <si>
+    <t>4:37
+em resumo: "th:object" e o "th:field" são capazes de instanciar um objeto de entidade/banco de dados e setar os seus atributos de acordo com os valores dos elementos HTML e entregar os dados para o Controller da aplicação.</t>
+  </si>
+  <si>
+    <t>6:58
+uma excessão que vale a pena comentar, pois é sobre o fato de ter declarado um th:object na pagina HTML de cadastro de Departamentos porém não foi declarado no endpoint, ou seja, ao chamar o endpoint, gera este erro. A solução é declarar tbm em forma de parametro no metodo do endpoint.</t>
   </si>
 </sst>
 </file>
@@ -567,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E25"/>
+  <dimension ref="B2:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,6 +942,76 @@
         <v>50</v>
       </c>
     </row>
+    <row r="26" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B26" s="3">
+        <v>36</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B27" s="3">
+        <v>36</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B28" s="3">
+        <v>36</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B29" s="3">
+        <v>36</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B30" s="3">
+        <v>36</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aula 37 - Listando departamentos
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="61">
   <si>
     <t>aula</t>
   </si>
@@ -259,12 +259,49 @@
     <t>6:58
 uma excessão que vale a pena comentar, pois é sobre o fato de ter declarado um th:object na pagina HTML de cadastro de Departamentos porém não foi declarado no endpoint, ou seja, ao chamar o endpoint, gera este erro. A solução é declarar tbm em forma de parametro no metodo do endpoint.</t>
   </si>
+  <si>
+    <t>37. Listando departamentos</t>
+  </si>
+  <si>
+    <t>1:28
+aplicando "for each" no thymeleaf para preencher tabelas HTML:
+th:each="nomeVariavelQlqr : ${nomeVariavelIdenticaAoController}"
+nomeVariavelQlqr: representa a linha referente a posição do for que está
+nomeVariavelIdenticaAoController: será a variável que conterá a lista recebida do controller/backend</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4:03
+abordado um dos três conceitos principais no </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Spring MVC - o Model  (os 3 são Model , ModelMap e o ModelAndView)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> para renderizar e construir páginas HTML com dados do controller.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,6 +313,12 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -301,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -311,6 +354,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -593,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E30"/>
+  <dimension ref="B2:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,6 +1059,34 @@
         <v>57</v>
       </c>
     </row>
+    <row r="31" spans="2:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="B31" s="5">
+        <v>37</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B32" s="5">
+        <v>37</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aula 38 - Editando departamentos
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
   <si>
     <t>aula</t>
   </si>
@@ -293,15 +293,40 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> para renderizar e construir páginas HTML com dados do controller.</t>
+      <t xml:space="preserve"> para renderizar e construir páginas HTML com dados do controller.
+Mais infos: </t>
     </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://www.baeldung.com/spring-mvc-model-model-map-model-view</t>
+    </r>
+  </si>
+  <si>
+    <t>38. Editando depatamentos</t>
+  </si>
+  <si>
+    <t>4:22
+um teste condicional direto no documento HTML para testar variavel se for null SALVA um novo objeto se conter algum valor ele EDITA o objeto valorado.
+th:action="${departamento.id == null} ? @{/departamentos/salvar} : @{/departamentos/editar}"</t>
+  </si>
+  <si>
+    <t>7:29
+aborda como captar o item selecionado de uma table HTML e atribuir o valor de algum dado contido nela a uma variavel declarada direto no documento HTML
+"@{/departamentos/editar/{idObj}(idObj=${nomeVariavelQlqr.id})}"
+onde nomeVariavelQlqr foi declarada em aulas anteriores. Ela armazena o itel atual do loop for-each</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -319,6 +344,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -640,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E32"/>
+  <dimension ref="B2:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,7 +1105,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" ht="105" x14ac:dyDescent="0.25">
       <c r="B32" s="5">
         <v>37</v>
       </c>
@@ -1086,6 +1118,40 @@
       <c r="E32" s="1" t="s">
         <v>60</v>
       </c>
+    </row>
+    <row r="33" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="B33" s="5">
+        <v>38</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="B34" s="5">
+        <v>38</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Excluindo departamentos - (parte 1) apenas back-end nesta parte
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="66">
   <si>
     <t>aula</t>
   </si>
@@ -320,6 +320,13 @@
 aborda como captar o item selecionado de uma table HTML e atribuir o valor de algum dado contido nela a uma variavel declarada direto no documento HTML
 "@{/departamentos/editar/{idObj}(idObj=${nomeVariavelQlqr.id})}"
 onde nomeVariavelQlqr foi declarada em aulas anteriores. Ela armazena o itel atual do loop for-each</t>
+  </si>
+  <si>
+    <t>39. Excluindo departamentos</t>
+  </si>
+  <si>
+    <t>4:36
+abordado outra forma de retornar para outra página a partir do controller sem usar o REDIRECT. Invés disso, pode ser usado algum método get do controller, como por exemplo, os metodos de listar todos</t>
   </si>
 </sst>
 </file>
@@ -675,7 +682,7 @@
   <dimension ref="B2:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,11 +1154,19 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
+    <row r="35" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B35" s="5">
+        <v>39</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Aula 40 - Finalizando a acao de exclusao - testado e funcionando
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="71">
   <si>
     <t>aula</t>
   </si>
@@ -327,6 +327,27 @@
   <si>
     <t>4:36
 abordado outra forma de retornar para outra página a partir do controller sem usar o REDIRECT. Invés disso, pode ser usado algum método get do controller, como por exemplo, os metodos de listar todos</t>
+  </si>
+  <si>
+    <t>2:14
+8. Departamento: Controller &amp; View
+40. Finalizando a ação de exclusão
+transformando o modal em um fragment com th:fragment</t>
+  </si>
+  <si>
+    <t>40. Finalizando a ação de exclusão</t>
+  </si>
+  <si>
+    <t>0:48
+primeiro uso de MODAL (um componente do bootstrap) no projeto. Uma espécie de janela de confirmação antes de excluir um departamento.</t>
+  </si>
+  <si>
+    <t>5:05
+primeira abordagem de javascrpit no projeto, para trabalhar com o botao de excluir na lista de departamentos.</t>
+  </si>
+  <si>
+    <t>10:53
+em resumo, na aula 40 implementamos o botão de excluir no frontend, construimos um fragmento de pagina MODAL modelo de confirmação de exclusão antes de excluir o objeto da lista, onde a exclusão de fato do objeto acontece ao clicar em OK na mensagem, ou seja, a requisição URL de deletar acontecer ao CONFIRMAR no modal.</t>
   </si>
 </sst>
 </file>
@@ -679,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E35"/>
+  <dimension ref="B2:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,6 +1189,62 @@
         <v>65</v>
       </c>
     </row>
+    <row r="36" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B36" s="5">
+        <v>40</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B37" s="5">
+        <v>40</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B38" s="5">
+        <v>40</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="B39" s="5">
+        <v>40</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aula 41 - Alerta de Sucesso
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="74">
   <si>
     <t>aula</t>
   </si>
@@ -349,12 +349,49 @@
     <t>10:53
 em resumo, na aula 40 implementamos o botão de excluir no frontend, construimos um fragmento de pagina MODAL modelo de confirmação de exclusão antes de excluir o objeto da lista, onde a exclusão de fato do objeto acontece ao clicar em OK na mensagem, ou seja, a requisição URL de deletar acontecer ao CONFIRMAR no modal.</t>
   </si>
+  <si>
+    <t>41. Alerta de sucesso</t>
+  </si>
+  <si>
+    <t>3:32
+para exibir os alerts, é o controller no back-end que envia as variaveis para as páginas, que no caso são mensagens de SUCESS ou FAIL de acordo com o comportamento dos métidos inserir, editar ou excluir. A implementação fica a critério.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4:50
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IMPORTANTISSIMO:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  ao enviar variaveis EL para o front-end:
+se usar o redirect para retornar para uma pagina, no escopo do método deve usar um parametro "RedirectAttributes" passando variavel EL para o front com o metodo "addFlashAttributes"
+se usar o ModelMap para retornar uma pagina, no escopo do método deve usar um parametro ModelMap passando a variavel EL para o front com o método "addAttribute"</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -383,13 +420,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -404,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -418,6 +477,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -700,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E39"/>
+  <dimension ref="B2:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1245,6 +1307,40 @@
         <v>70</v>
       </c>
     </row>
+    <row r="40" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B40" s="5">
+        <v>41</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="189" x14ac:dyDescent="0.25">
+      <c r="B41" s="5">
+        <v>41</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E43" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aulas 43 e 44 - Inserindo Cargos e Conversor para Departamento
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="81">
   <si>
     <t>aula</t>
   </si>
@@ -386,12 +386,85 @@
 se usar o ModelMap para retornar uma pagina, no escopo do método deve usar um parametro ModelMap passando a variavel EL para o front com o método "addAttribute"</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t>4:51</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (CONTEUDO ABAIXO FOI UMA PESQUISA, FORA DA AULA)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Uma das anotações mais importantes do Spring-MVC é a anotação @ModelAttribute .
+O @ModelAttribute é uma anotação que vincula um parâmetro de método ou valor de retorno de método a um atributo de modelo nomeado e o expõe a uma visualização da web.
+@ModelAttribute 
+public void addAttributes(Model model) { 
+     model.addAttribute("msg", "Welcome to the Netherlands!");
+ }
+Em geral, Spring-MVC sempre fará uma chamada primeiro para esse método, antes de chamar qualquer método do manipulador de solicitação. Ou seja, os métodos @ModelAttribute são chamados antes dos métodos do controlador anotados com @RequestMapping serem chamados. A lógica por trás da sequência é que, o objeto de modelo deve ser criado antes que qualquer processamento seja iniciado dentro dos métodos do controlador.Quando usado como um argumento do método, indica que o argumento deve ser recuperado do modelo. Quando não estiver presente, ele deve ser instanciado primeiro e, em seguida, adicionado ao modelo e, uma vez presente no modelo, os campos de argumentos devem ser preenchidos a partir de todos os parâmetros de solicitação que possuem nomes correspondentes.
+@RequestMapping(value = "/addEmployee", method = RequestMethod.POST) 
+public String submit(@ModelAttribute("employee") Employee employee) { 
+// Code that uses the employee object 
+return "employeeView"; 
+}
+mais infos:
+https://www.baeldung.com/spring-mvc-and-the-modelattribute-annotation</t>
+    </r>
+  </si>
+  <si>
+    <t>9. Cargo: Controller &amp; View</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+3:01
+quando hà relações, é necessário injetar também as depêndencias das entidades relacionadas</t>
+  </si>
+  <si>
+    <t>43. Inserindo cargos</t>
+  </si>
+  <si>
+    <t>44. Conversor para Departamento</t>
+  </si>
+  <si>
+    <t>5:40
+ao injetar objetos, a classe deve ser transformada em um Bean gerenciado pelo spring e no caso, foi usado a anotação @Component</t>
+  </si>
+  <si>
+    <t>1:36
+criação de classe para conversão de dados/entidades recebidas do frontend. (Ex.: relacionamentos de entidades).Primeira abordagem da interface Converter do spring, que auxilia na conversão.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -432,6 +505,14 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -762,17 +843,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E43"/>
+  <dimension ref="B2:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="39.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="74.140625" customWidth="1"/>
+    <col min="5" max="5" width="158.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
@@ -817,7 +898,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>10</v>
       </c>
@@ -831,7 +912,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>11</v>
       </c>
@@ -873,7 +954,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" ht="105" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>14</v>
       </c>
@@ -887,7 +968,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>15</v>
       </c>
@@ -901,7 +982,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>16</v>
       </c>
@@ -915,7 +996,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>17</v>
       </c>
@@ -929,7 +1010,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>22</v>
       </c>
@@ -943,7 +1024,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>24</v>
       </c>
@@ -957,7 +1038,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>25</v>
       </c>
@@ -971,7 +1052,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>27</v>
       </c>
@@ -985,7 +1066,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>29</v>
       </c>
@@ -1013,7 +1094,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>30</v>
       </c>
@@ -1027,7 +1108,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>31</v>
       </c>
@@ -1041,7 +1122,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>32</v>
       </c>
@@ -1055,7 +1136,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="2:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>32</v>
       </c>
@@ -1069,7 +1150,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>33</v>
       </c>
@@ -1111,7 +1192,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <v>36</v>
       </c>
@@ -1125,7 +1206,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <v>36</v>
       </c>
@@ -1139,7 +1220,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <v>36</v>
       </c>
@@ -1153,7 +1234,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <v>36</v>
       </c>
@@ -1167,7 +1248,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <v>36</v>
       </c>
@@ -1181,7 +1262,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="2:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" ht="105" x14ac:dyDescent="0.25">
       <c r="B31" s="5">
         <v>37</v>
       </c>
@@ -1195,7 +1276,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="2:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B32" s="5">
         <v>37</v>
       </c>
@@ -1237,7 +1318,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B35" s="5">
         <v>39</v>
       </c>
@@ -1251,7 +1332,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="5">
         <v>40</v>
       </c>
@@ -1279,7 +1360,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B38" s="5">
         <v>40</v>
       </c>
@@ -1293,7 +1374,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B39" s="5">
         <v>40</v>
       </c>
@@ -1307,7 +1388,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B40" s="5">
         <v>41</v>
       </c>
@@ -1321,7 +1402,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="2:5" ht="189" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:5" ht="157.5" x14ac:dyDescent="0.25">
       <c r="B41" s="5">
         <v>41</v>
       </c>
@@ -1335,11 +1416,61 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E43" s="1"/>
+    <row r="42" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="B42" s="5">
+        <v>43</v>
+      </c>
+      <c r="C42" t="s">
+        <v>75</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="390" x14ac:dyDescent="0.25">
+      <c r="B43" s="5">
+        <v>43</v>
+      </c>
+      <c r="C43" t="s">
+        <v>75</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B44" s="5">
+        <v>44</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B45" s="5">
+        <v>44</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Aula 47 - Excluindo cargos
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="83">
   <si>
     <t>aula</t>
   </si>
@@ -458,6 +458,14 @@
   <si>
     <t>1:36
 criação de classe para conversão de dados/entidades recebidas do frontend. (Ex.: relacionamentos de entidades).Primeira abordagem da interface Converter do spring, que auxilia na conversão.</t>
+  </si>
+  <si>
+    <t>47. Excluindo cargos</t>
+  </si>
+  <si>
+    <t>2:39
+nova forma de concatenar valores no documento HTML utilizando recursos do próprio thymeleaf
+th:id="${#strings.concat('btn_cargos/excluir/', nomeVariavelQlqr.id)}</t>
   </si>
 </sst>
 </file>
@@ -843,10 +851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E45"/>
+  <dimension ref="B2:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1472,6 +1480,20 @@
         <v>79</v>
       </c>
     </row>
+    <row r="46" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B46" s="5">
+        <v>47</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aulas 49 e 50 - Inserindo funcionarios e Conversores para funcionarios e correcao de bugs com Transactional
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="90">
   <si>
     <t>aula</t>
   </si>
@@ -466,6 +466,59 @@
     <t>2:39
 nova forma de concatenar valores no documento HTML utilizando recursos do próprio thymeleaf
 th:id="${#strings.concat('btn_cargos/excluir/', nomeVariavelQlqr.id)}</t>
+  </si>
+  <si>
+    <t>10. Funcionário: Controller &amp; View</t>
+  </si>
+  <si>
+    <t>49. Inserindo funcionários</t>
+  </si>
+  <si>
+    <t>4:27
+atenção a formatação de valores monetários. Necessário aplicar script/biblioteca javascript na página para utilizar mascaras aliada a tag data-mask="FORMATO_SUA_MASK_AQUI"</t>
+  </si>
+  <si>
+    <t>50. Conversores para funcionarios</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AVISO IMPORTANTE: se atentar a possivel erro de conversão monetario ou de calendario. Se a mascara estiver no formato PT-BR ... O idioma do sistema operacional também deve estar em PT-BR para funcionar. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MAIS INFOS NA AULA N° 56</t>
+    </r>
+  </si>
+  <si>
+    <t>50. Conversores para funcionários</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3:12
+aprendendo a converter dados (Ex. Moeda, Datas, etc...) usando propriedades do próprio spring nas classes de domínio. Para converter os dados, basta inserir anotações nos atributos da classe;
+@NumberFormat(style = Style.CURRENCY, pattern = "#,##0.00")
+ou
+@DateTimeFormat(iso = ISO.DATE)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IMPORTANTE: NumerFormat, foi usado uma mascara para padrao AMERICANO, e deve ser assim... já a máscara na view/front-end não precisa seguir esta regra, pode usar mascara PT-BR mesmo</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -851,10 +904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E46"/>
+  <dimension ref="B2:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1494,6 +1547,48 @@
         <v>82</v>
       </c>
     </row>
+    <row r="47" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B47" s="5">
+        <v>49</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" s="5">
+        <v>50</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" ht="180" x14ac:dyDescent="0.25">
+      <c r="B49" s="5">
+        <v>50</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aula 51 - Listando funcionarios
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="94">
   <si>
     <t>aula</t>
   </si>
@@ -519,6 +519,24 @@
       </rPr>
       <t>IMPORTANTE: NumerFormat, foi usado uma mascara para padrao AMERICANO, e deve ser assim... já a máscara na view/front-end não precisa seguir esta regra, pode usar mascara PT-BR mesmo</t>
     </r>
+  </si>
+  <si>
+    <t>1:27
+formatação de valores monetários na página HTML usando a expressão com pipes;
+|R$ ${{nomeVariavelQlqr.seuAtributoValor}}|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+51. Listando funcionários</t>
+  </si>
+  <si>
+    <t>4:39
+o popover precisa de recursos das bibliotecas do bootstrap e de componentes javascript. ele precisa de tags HTML como data-container ... data-toggle, data-placement e data-content ... mas como o thymeleaf não tem componentes próprios para substituir estas tags, então é usado o "th:attr" que implementa de forma genérica as tags necessárias.</t>
+  </si>
+  <si>
+    <t>6:13
+formatando datas no HTML com temporals.format do pacote java.time;
+th:text="${#temporals.format(nomeVariavelQlqr.data, 'dd/MM/yyyy')}"</t>
   </si>
 </sst>
 </file>
@@ -904,10 +922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E49"/>
+  <dimension ref="B2:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56:E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1589,6 +1607,53 @@
         <v>89</v>
       </c>
     </row>
+    <row r="50" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B50" s="5">
+        <v>50</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B51" s="5">
+        <v>50</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B52" s="5">
+        <v>50</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aula 53 - Buscar funcionario por nome
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="97">
   <si>
     <t>aula</t>
   </si>
@@ -537,6 +537,21 @@
     <t>6:13
 formatando datas no HTML com temporals.format do pacote java.time;
 th:text="${#temporals.format(nomeVariavelQlqr.data, 'dd/MM/yyyy')}"</t>
+  </si>
+  <si>
+    <t>5:27
+interessante: foi demonstrado o tanto de código necessário para efetuar uma consulta JPQL e como evitar isso usando um método ja criado anteriormente na aula 21 onde foi implementada uma classe abstrata e genérica AbstractDao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+53. Buscar funcionário por nome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1:54
+anotação @RequestParam  tem mesma usabilidade que o @PathVariable porém com diferenças:
+@RequestParam faz troca de valores e variaveis entre controller e view através da Request/Requisição de forma CODIFICADA. podemos ter vários parametros passados por url mas que não são parte da url em sí.
+@PathVariable faz troca de valores e variaveis entre controller e view através da path URL e NÃO CODIFICADO. Em resumo, o @PathVariable é utilizado quando o valor da variável é passada diretamente na URL, mas não como um parametro que você passa após o sinal de interrogação (?) mas sim quando o valor faz parte da url</t>
   </si>
 </sst>
 </file>
@@ -922,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E53"/>
+  <dimension ref="B2:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56:E58"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1609,7 +1624,7 @@
     </row>
     <row r="50" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B50" s="5">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>83</v>
@@ -1623,7 +1638,7 @@
     </row>
     <row r="51" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B51" s="5">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>83</v>
@@ -1637,7 +1652,7 @@
     </row>
     <row r="52" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B52" s="5">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>83</v>
@@ -1649,10 +1664,33 @@
         <v>93</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="1"/>
+    <row r="53" spans="2:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="B53" s="5">
+        <v>53</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B54" s="5">
+        <v>53</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>94</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Aula 55 - Buscar funcionario por datas
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="100">
   <si>
     <t>aula</t>
   </si>
@@ -552,6 +552,23 @@
 anotação @RequestParam  tem mesma usabilidade que o @PathVariable porém com diferenças:
 @RequestParam faz troca de valores e variaveis entre controller e view através da Request/Requisição de forma CODIFICADA. podemos ter vários parametros passados por url mas que não são parte da url em sí.
 @PathVariable faz troca de valores e variaveis entre controller e view através da path URL e NÃO CODIFICADO. Em resumo, o @PathVariable é utilizado quando o valor da variável é passada diretamente na URL, mas não como um parametro que você passa após o sinal de interrogação (?) mas sim quando o valor faz parte da url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+55. Buscar funcionário por datas</t>
+  </si>
+  <si>
+    <t>5:15
+INTERESSANTE: uso de varargs ...
+O professor não explica mas na aula ele utiliza o metodo createQuery com varios parâmetros, sendo que na assinatura do métido está Object ... params .
+Pesquisando no google, compreendi que se usa varargs quando não sabe quantos de um determinado tipo de argumento/parâmetros serão passados ​​para o método.
+mais infos:
+https://docs.oracle.com/javase/tutorial/java/javaOO/arguments.html</t>
+  </si>
+  <si>
+    <t>6:33
+Convertendo datas do formulario/view/doc HTML em um formato LocalDate para que o controller não gere erro.
+para converter, adicionar a anotação @DateTimeFormat(iso = DateTimeFormat.ISO.DATE)  no parametro do método no controller.</t>
   </si>
 </sst>
 </file>
@@ -937,10 +954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E54"/>
+  <dimension ref="B2:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1692,6 +1709,34 @@
         <v>94</v>
       </c>
     </row>
+    <row r="55" spans="2:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="B55" s="5">
+        <v>55</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B56" s="5">
+        <v>55</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aula 57 - Validando formulario de cargo e departamento
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\CURSO - SPRING BOOT, IONIC\workspace sts 2 (migrando repositorio github)\curso_spring_boot_MVC_com_thymeleaf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\java\curso-spring-MVC-thymeleaf\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="107">
   <si>
     <t>aula</t>
   </si>
@@ -569,6 +569,43 @@
     <t>6:33
 Convertendo datas do formulario/view/doc HTML em um formato LocalDate para que o controller não gere erro.
 para converter, adicionar a anotação @DateTimeFormat(iso = DateTimeFormat.ISO.DATE)  no parametro do método no controller.</t>
+  </si>
+  <si>
+    <t>0:44
+começando sessão de validação dos campos. Para isso é necessário trabalhar com Bean Validation ... requer dependencia:
+&lt;!-- TOMAR CUIIDADO COM VERSÃO DO SPRING BOOT, A DEPENDENCIA ABAIXO
+ATENDE AS VERSÕES DO SPRING ACIMA DE 2.3.0 --&gt;
+&lt;dependency&gt;
+ &lt;groupId&gt;org.springframework.boot&lt;/groupId&gt;
+ &lt;artifactId&gt;spring-boot-starter-validation&lt;/artifactId&gt;
+&lt;/dependency&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+57. Validando formulários de cargo e departamento</t>
+  </si>
+  <si>
+    <t>11. Validação Back-End</t>
+  </si>
+  <si>
+    <t>1:12
+anotações utilizadas no domain para validação dos seus atributos:
+@NotBlank(message="")
+@Size()</t>
+  </si>
+  <si>
+    <t>6:33
+anotação @Valid nos métodos salvar e editar para validar campos entre controller e view HTML</t>
+  </si>
+  <si>
+    <t>6:56
+adicionado um parametro do tipo BindingResult do spring para trabalhar em conjunto com a anotação @Valid nas validaçoes dos campos</t>
+  </si>
+  <si>
+    <t>5:36
+IMPORTANTE: PARA FUNCIONAR DEVE ESTAR DENTRO DE UMA TAG "FORM" NO HTML caso contrário não funcionará.
+inclusão de fragmento de validação de campos nos forms de cadastro de departamento e de cargos para mostrar mensagens na tela.
+&lt;div th:replace="fragments/validacao :: validacao"&gt;&lt;/div&gt;</t>
   </si>
 </sst>
 </file>
@@ -954,10 +991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E56"/>
+  <dimension ref="B2:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1737,6 +1774,76 @@
         <v>99</v>
       </c>
     </row>
+    <row r="57" spans="2:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="B57" s="5">
+        <v>57</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B58" s="5">
+        <v>57</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="B59" s="5">
+        <v>57</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B60" s="5">
+        <v>57</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B61" s="5">
+        <v>57</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aula 58 e 59 - Validando funcionario e endereco e Validando campo a campo funcionarios
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="112">
   <si>
     <t>aula</t>
   </si>
@@ -606,6 +606,27 @@
 IMPORTANTE: PARA FUNCIONAR DEVE ESTAR DENTRO DE UMA TAG "FORM" NO HTML caso contrário não funcionará.
 inclusão de fragmento de validação de campos nos forms de cadastro de departamento e de cargos para mostrar mensagens na tela.
 &lt;div th:replace="fragments/validacao :: validacao"&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+58. Validando funcionário e endereço</t>
+  </si>
+  <si>
+    <t>0:24
+armazenando mensagens de validação dos campos direto em um arquivo .properties. Deve ser inserido no classpath da aplicação
+uma forma diferente de lidar com as anotações @NotNull , @NotBlank , @Size</t>
+  </si>
+  <si>
+    <t>3:50
+IMPORTANTE: uso da anotação @Valid diretamento no atribut do dominio invés do controller. Neste caso especifico ela foi aplicada em um atributo que tem relação com outras tabelas, sendo assim, as validaçoes que serão aplicadas serão as que estao configuradas do outro lado da entidade.</t>
+  </si>
+  <si>
+    <t>0:43
+uso do th:classappend para validação de formulários campo a campo. permite efetuar a troca do tipo de classe no documento HTML em tempo de execução. faz o componente que foi invalidado ficar com a borda avermelhada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+59. Validação campo a campo para funcionário</t>
   </si>
 </sst>
 </file>
@@ -991,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E61"/>
+  <dimension ref="B2:E64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1844,6 +1865,48 @@
         <v>105</v>
       </c>
     </row>
+    <row r="62" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B62" s="5">
+        <v>58</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B63" s="5">
+        <v>58</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B64" s="5">
+        <v>59</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aula 60 - Validacao de data com Spring Validator (Importante para Regras de Negocio)
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\java\curso-spring-MVC-thymeleaf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\CURSO - SPRING BOOT, IONIC\workspace sts 2 (migrando repositorio github)\curso-spring-MVC-thymeleaf\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="116">
   <si>
     <t>aula</t>
   </si>
@@ -627,6 +627,25 @@
   <si>
     <t xml:space="preserve">
 59. Validação campo a campo para funcionário</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+60. Validação de data com Spring Validator</t>
+  </si>
+  <si>
+    <t>8:21
+anotação @InitBinder : está anotação diz para a aplicação que este método sera o primeiro metodo da classe que vai ser executado ao ser chamado FuncionarioController. Desta forma, ao ser executado, o SPring MVC vai até a classe FuncionarioValidator fazer a validação antes de liberar o acesso a requisição pra os metodos salvar e editar</t>
+  </si>
+  <si>
+    <t>10:22
+IMPORTANTE - REGRAS DE NEGÓCIO E VALIDAÇÃO: no metodo validate() pode conter qualquer tipo de validação de campos HTML, perfeito para validar as regras de negócio da aplicação.</t>
+  </si>
+  <si>
+    <t>7:11
+a criação do arquivo messages.properties é devido a especificação do Spring Validator
+e o arquivo ValidationMessages.Properties é um arquivo próprio
+da especificação Bean Validation, que automaticamente já procura este arquivo no classpath
+o Spring Validation foi criado antes do Bean validation</t>
   </si>
 </sst>
 </file>
@@ -713,7 +732,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -730,6 +749,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1012,10 +1034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E64"/>
+  <dimension ref="B2:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1907,6 +1929,48 @@
         <v>110</v>
       </c>
     </row>
+    <row r="65" spans="2:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="B65" s="5">
+        <v>60</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B66" s="5">
+        <v>60</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B67" s="5">
+        <v>60</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aula 61 - Convertendo String para Integer e validando
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="118">
   <si>
     <t>aula</t>
   </si>
@@ -647,12 +647,18 @@
 da especificação Bean Validation, que automaticamente já procura este arquivo no classpath
 o Spring Validation foi criado antes do Bean validation</t>
   </si>
+  <si>
+    <t>61. Convertendo String para Integer e Validando</t>
+  </si>
+  <si>
+    <t>criado uma classe StringToInteger para validar o campo de "numero de endereço" proibindo salvar ou submeter o formulario caso o usuario digite letras no campo de numero</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -705,6 +711,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -732,7 +746,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -754,6 +768,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1034,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E67"/>
+  <dimension ref="B2:E70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1971,6 +1986,23 @@
         <v>114</v>
       </c>
     </row>
+    <row r="68" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B68" s="5">
+        <v>61</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E70" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aula 63 - Nomeando os componentes do HTML
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="120">
   <si>
     <t>aula</t>
   </si>
@@ -652,6 +652,12 @@
   </si>
   <si>
     <t>criado uma classe StringToInteger para validar o campo de "numero de endereço" proibindo salvar ou submeter o formulario caso o usuario digite letras no campo de numero</t>
+  </si>
+  <si>
+    <t>63. Nomeando os componentes do HTML</t>
+  </si>
+  <si>
+    <t>foi abordado como nomear os componentes HTML através do arquivo messages.properties. Uma boa forma de centralizar os titulos de pagina HTML dos componentes, cabeçalhos de tabelas, etc</t>
   </si>
 </sst>
 </file>
@@ -1051,8 +1057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2000,6 +2006,20 @@
         <v>117</v>
       </c>
     </row>
+    <row r="69" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B69" s="5">
+        <v>63</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E70" s="9"/>
     </row>

</xml_diff>

<commit_message>
Aula 66 - Manipulando a pagina de erro
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\java\curso-spring-MVC-thymeleaf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\CURSO - SPRING BOOT, IONIC\workspace sts 2 (migrando repositorio github)\curso-spring-MVC-thymeleaf\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="125">
   <si>
     <t>aula</t>
   </si>
@@ -670,12 +670,19 @@
 inclusão de nova pagina HTML chamada error.html, para tratar os erros da aplicação.
 o nome dado ao documento HTML "error.html" é um padrão utilizado pelo thymeleaf para reconhecer no classpath "templates"</t>
   </si>
+  <si>
+    <t>66. Manipulando página de erro</t>
+  </si>
+  <si>
+    <t>1:15
+criação de classe MyErrorView para manipular a página padrão de erros do thymeleaf</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -728,6 +735,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -755,7 +767,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -777,6 +789,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -836,8 +849,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:D69" totalsRowShown="0">
-  <autoFilter ref="A1:D69"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:D70" totalsRowShown="0">
+  <autoFilter ref="A1:D70"/>
   <tableColumns count="4">
     <tableColumn id="1" name="aula" dataDxfId="3"/>
     <tableColumn id="2" name="sessão" dataDxfId="2"/>
@@ -1113,18 +1126,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="39.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="158.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1138,7 +1151,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>9</v>
       </c>
@@ -1152,7 +1165,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="45">
       <c r="A3">
         <v>10</v>
       </c>
@@ -1166,7 +1179,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="45">
       <c r="A4">
         <v>10</v>
       </c>
@@ -1180,7 +1193,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="45">
       <c r="A5">
         <v>11</v>
       </c>
@@ -1194,7 +1207,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>12</v>
       </c>
@@ -1208,7 +1221,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>13</v>
       </c>
@@ -1222,7 +1235,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="105">
       <c r="A8">
         <v>14</v>
       </c>
@@ -1236,7 +1249,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="30">
       <c r="A9">
         <v>15</v>
       </c>
@@ -1250,7 +1263,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="30">
       <c r="A10">
         <v>16</v>
       </c>
@@ -1264,7 +1277,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="30">
       <c r="A11">
         <v>17</v>
       </c>
@@ -1278,7 +1291,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>22</v>
       </c>
@@ -1292,7 +1305,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="60">
       <c r="A13" s="3">
         <v>24</v>
       </c>
@@ -1306,7 +1319,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>25</v>
       </c>
@@ -1320,7 +1333,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>27</v>
       </c>
@@ -1334,7 +1347,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="60">
       <c r="A16">
         <v>29</v>
       </c>
@@ -1348,7 +1361,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="105">
       <c r="A17">
         <v>29</v>
       </c>
@@ -1362,7 +1375,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="60">
       <c r="A18">
         <v>30</v>
       </c>
@@ -1376,7 +1389,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="75">
       <c r="A19">
         <v>31</v>
       </c>
@@ -1390,7 +1403,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>32</v>
       </c>
@@ -1404,7 +1417,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="75">
       <c r="A21">
         <v>32</v>
       </c>
@@ -1418,7 +1431,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="30">
       <c r="A22">
         <v>33</v>
       </c>
@@ -1432,7 +1445,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="30">
       <c r="A23">
         <v>34</v>
       </c>
@@ -1446,7 +1459,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="45">
       <c r="A24">
         <v>35</v>
       </c>
@@ -1460,7 +1473,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="45">
       <c r="A25" s="3">
         <v>36</v>
       </c>
@@ -1474,7 +1487,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="45">
       <c r="A26" s="3">
         <v>36</v>
       </c>
@@ -1488,7 +1501,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="45">
       <c r="A27" s="3">
         <v>36</v>
       </c>
@@ -1502,7 +1515,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="45">
       <c r="A28" s="3">
         <v>36</v>
       </c>
@@ -1516,7 +1529,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="45">
       <c r="A29" s="3">
         <v>36</v>
       </c>
@@ -1530,7 +1543,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="105">
       <c r="A30" s="5">
         <v>37</v>
       </c>
@@ -1544,7 +1557,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="75">
       <c r="A31" s="5">
         <v>37</v>
       </c>
@@ -1558,7 +1571,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="60">
       <c r="A32" s="5">
         <v>38</v>
       </c>
@@ -1572,7 +1585,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="90">
       <c r="A33" s="5">
         <v>38</v>
       </c>
@@ -1586,7 +1599,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="45">
       <c r="A34" s="5">
         <v>39</v>
       </c>
@@ -1600,7 +1613,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="30">
       <c r="A35" s="5">
         <v>40</v>
       </c>
@@ -1614,7 +1627,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="60">
       <c r="A36" s="5">
         <v>40</v>
       </c>
@@ -1628,7 +1641,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="30">
       <c r="A37" s="5">
         <v>40</v>
       </c>
@@ -1642,7 +1655,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="45">
       <c r="A38" s="5">
         <v>40</v>
       </c>
@@ -1656,7 +1669,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="45">
       <c r="A39" s="5">
         <v>41</v>
       </c>
@@ -1670,7 +1683,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="157.5">
       <c r="A40" s="5">
         <v>41</v>
       </c>
@@ -1684,7 +1697,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="90">
       <c r="A41" s="5">
         <v>43</v>
       </c>
@@ -1698,7 +1711,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="390" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="390">
       <c r="A42" s="5">
         <v>43</v>
       </c>
@@ -1712,7 +1725,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="45">
       <c r="A43" s="5">
         <v>44</v>
       </c>
@@ -1726,7 +1739,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="30">
       <c r="A44" s="5">
         <v>44</v>
       </c>
@@ -1740,7 +1753,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="60">
       <c r="A45" s="5">
         <v>47</v>
       </c>
@@ -1754,7 +1767,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="45">
       <c r="A46" s="5">
         <v>49</v>
       </c>
@@ -1768,7 +1781,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="30">
       <c r="A47" s="5">
         <v>50</v>
       </c>
@@ -1782,7 +1795,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="180" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="180">
       <c r="A48" s="5">
         <v>50</v>
       </c>
@@ -1796,7 +1809,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="75">
       <c r="A49" s="5">
         <v>51</v>
       </c>
@@ -1810,7 +1823,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="60">
       <c r="A50" s="5">
         <v>51</v>
       </c>
@@ -1824,7 +1837,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="60">
       <c r="A51" s="5">
         <v>51</v>
       </c>
@@ -1838,7 +1851,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="165">
       <c r="A52" s="5">
         <v>53</v>
       </c>
@@ -1852,7 +1865,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="60">
       <c r="A53" s="5">
         <v>53</v>
       </c>
@@ -1866,7 +1879,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="150">
       <c r="A54" s="5">
         <v>55</v>
       </c>
@@ -1880,7 +1893,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="75">
       <c r="A55" s="5">
         <v>55</v>
       </c>
@@ -1894,7 +1907,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="165">
       <c r="A56" s="5">
         <v>57</v>
       </c>
@@ -1908,7 +1921,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="75">
       <c r="A57" s="5">
         <v>57</v>
       </c>
@@ -1922,7 +1935,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="90">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -1936,7 +1949,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="45">
       <c r="A59" s="5">
         <v>57</v>
       </c>
@@ -1950,7 +1963,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="45">
       <c r="A60" s="5">
         <v>57</v>
       </c>
@@ -1964,7 +1977,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="75">
       <c r="A61" s="5">
         <v>58</v>
       </c>
@@ -1978,7 +1991,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" ht="45">
       <c r="A62" s="5">
         <v>58</v>
       </c>
@@ -1992,7 +2005,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="60">
       <c r="A63" s="5">
         <v>59</v>
       </c>
@@ -2006,7 +2019,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="120">
       <c r="A64" s="5">
         <v>60</v>
       </c>
@@ -2020,7 +2033,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="45">
       <c r="A65" s="5">
         <v>60</v>
       </c>
@@ -2034,7 +2047,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="45">
       <c r="A66" s="5">
         <v>60</v>
       </c>
@@ -2048,7 +2061,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="30">
       <c r="A67" s="5">
         <v>61</v>
       </c>
@@ -2062,7 +2075,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="30">
       <c r="A68" s="5">
         <v>63</v>
       </c>
@@ -2076,7 +2089,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="75">
       <c r="A69" s="5">
         <v>65</v>
       </c>
@@ -2090,8 +2103,19 @@
         <v>122</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D70" s="1"/>
+    <row r="70" spans="1:4" ht="45">
+      <c r="A70" s="9">
+        <v>66</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Aula 68 - Padronizando as URLs internas
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="128">
   <si>
     <t>aula</t>
   </si>
@@ -676,6 +676,19 @@
   <si>
     <t>1:15
 criação de classe MyErrorView para manipular a página padrão de erros do thymeleaf</t>
+  </si>
+  <si>
+    <t>1:34
+substituido todas links e tags href e src que apontam para as paginas HTML da aplicação pelo padrão do thymeleaf:
+th:href="@{/suapaginaaqui}
+th:src="@{/seucaminhoaqui}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+68. Padronizando as URLs internas</t>
+  </si>
+  <si>
+    <t>14. Final</t>
   </si>
 </sst>
 </file>
@@ -849,8 +862,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:D70" totalsRowShown="0">
-  <autoFilter ref="A1:D70"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:D71" totalsRowShown="0">
+  <autoFilter ref="A1:D71"/>
   <tableColumns count="4">
     <tableColumn id="1" name="aula" dataDxfId="3"/>
     <tableColumn id="2" name="sessão" dataDxfId="2"/>
@@ -1124,7 +1137,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
       <selection activeCell="D71" sqref="D71"/>
@@ -2117,6 +2130,20 @@
         <v>124</v>
       </c>
     </row>
+    <row r="71" spans="1:4" ht="90">
+      <c r="A71" s="9">
+        <v>68</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aula 69 - Executando a aplicacao via .jar
</commit_message>
<xml_diff>
--- a/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
+++ b/anotacoes-curso spring boot MVC e Thymeleaf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="131">
   <si>
     <t>aula</t>
   </si>
@@ -689,6 +689,17 @@
   </si>
   <si>
     <t>14. Final</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+69. Executando a aplicação via .jar</t>
+  </si>
+  <si>
+    <t>6:43
+em ações que não são do tipo "redirect" é preciso retirar a barra "/" no inicio de cada link existente na aplicação pois gera erro/conflito de path entre o Thymeleaf e o Spring boot ao executar o app diretamente pelo .jar</t>
+  </si>
+  <si>
+    <t>para executar a aplicação fora da IDE é necessário empacotar as classes executando e fazendo build através do maven e em "goals" adicionar o "package -e" para que seja criado o arquivo .jar na pasta target da aplicação. Após o arquivo criado, basta executalo pelo cmd atraves do comando "java -jar nomeDaSuaAplicacao.jar" (sem aspas)</t>
   </si>
 </sst>
 </file>
@@ -862,8 +873,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:D71" totalsRowShown="0">
-  <autoFilter ref="A1:D71"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:D73" totalsRowShown="0">
+  <autoFilter ref="A1:D73"/>
   <tableColumns count="4">
     <tableColumn id="1" name="aula" dataDxfId="3"/>
     <tableColumn id="2" name="sessão" dataDxfId="2"/>
@@ -1137,10 +1148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2144,6 +2155,34 @@
         <v>125</v>
       </c>
     </row>
+    <row r="72" spans="1:4" ht="30">
+      <c r="A72" s="9">
+        <v>69</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="60">
+      <c r="A73" s="9">
+        <v>69</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>